<commit_message>
elo elo działa trzeba uzywac lepszego modelu
</commit_message>
<xml_diff>
--- a/wyniki/1.xlsx
+++ b/wyniki/1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,21 @@
           <t>Maksymalny wynik</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Nazwa Pliku i rozdział</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Wynik</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Maksymalny Wynik</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,14 +499,15 @@
           <t>zdrowie, moje</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E2" t="n">
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
       </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -502,19 +518,21 @@
           <t>próżność, repliki, się, spodziewał, nie</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>ojczyzno, prztyczka, Litwo, ojczyzno, prztyczka</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>
       </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -535,14 +553,15 @@
           <t>jak, zdrowie</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="E4" t="n">
+        <v>5</v>
       </c>
       <c r="F4" t="n">
         <v>5</v>
       </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -563,14 +582,15 @@
           <t>ty</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E5" t="n">
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
       </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -591,14 +611,15 @@
           <t>ty, ojczyzno, jesteś</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E6" t="n">
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>5</v>
       </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -619,14 +640,15 @@
           <t>Częstochowy, broni</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E7" t="n">
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
       </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -647,14 +669,15 @@
           <t>jasne, br</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E8" t="n">
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
       </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -675,14 +698,15 @@
           <t>zdrowie</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E9" t="n">
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>
       </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -703,14 +727,15 @@
           <t>jak, zdrowie</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="E10" t="n">
+        <v>5</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
       </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -731,14 +756,15 @@
           <t>ojczyzną</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E11" t="n">
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>5</v>
       </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -759,13 +785,154 @@
           <t>pan</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E12" t="n">
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>5</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Piękne,  przykładem</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>przykładem.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Piękne,  przykładem</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>TAYLOR__Mechanika16k.wav</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Piękne,  przykładem</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>przykładem.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Piękne,  przykładem</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>TAYLOR__Mechanika16k.wav</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1/2</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> się,  ono,  odepchnąć,,  lub,  który,  mógłby,  ciało</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ono</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ciało,  mógłby,  ono,  się,  który,  lub,  odepchnąć,</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>TAYLOR__Mechanika16k.wav</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1/7</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> się,  ono,  odepchnąć,,  lub,  który,  mógłby,  ciało</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ono</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ciało,  mógłby,  ono,  się,  który,  lub,  odepchnąć,</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>TAYLOR__Mechanika16k.wav</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>1/7</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>